<commit_message>
Round-2 Feedback: Modification started
</commit_message>
<xml_diff>
--- a/Table_raw/LEBA Long.xlsx
+++ b/Table_raw/LEBA Long.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/mushfiqul_anwarsiraji_monash_edu/Documents/My papers/LEBA Common workplace/leba-manuscript/Table_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/mushfiqul_anwarsiraji_monash_edu/Documents/My papers/LEBA Common workplace/Instrument_distribution/instrument/Table_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{8ACCD78E-C453-334D-BEE0-9441604D48A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87D1FE41-22CF-9245-A680-E772C1180FC9}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{8ACCD78E-C453-334D-BEE0-9441604D48A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4123BD47-EC03-ED43-98E3-F00AFAA95B6E}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="1500" windowWidth="27640" windowHeight="16940" xr2:uid="{3D1EC2CC-B386-2E46-B2E3-D17B04FE0165}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{3D1EC2CC-B386-2E46-B2E3-D17B04FE0165}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,36 +54,12 @@
     <t>Always</t>
   </si>
   <si>
-    <t>01. I wear blue-filtering,orange-tinted,and/or red-tinted glasses indoors during the day.</t>
-  </si>
-  <si>
-    <t>02.  I wear blue-filtering, orange-tinted, and/or red-tinted glasses outdoors during the day.</t>
-  </si>
-  <si>
     <t>03. I wear blue-filtering, orange-tinted, and/or red-tinted glasses within 1 hour before attempting to fall asleep.</t>
   </si>
   <si>
-    <t>10.I use my mobile phone within 1 hour before attempting to fall asleep.</t>
-  </si>
-  <si>
-    <t>11.I look at my mobile phone screen immediately after waking up.</t>
-  </si>
-  <si>
     <t>12. I check my phone when I wake up at night.</t>
   </si>
   <si>
-    <t>13.I look at my smartwatch within 1 hour before attempting to fall asleep</t>
-  </si>
-  <si>
-    <t>14.I look at my smartwatch when I wake up at night.</t>
-  </si>
-  <si>
-    <t>15.I dim my mobile phone screen within 1 hour before attempting to fall asleep.</t>
-  </si>
-  <si>
-    <t>16.I use a blue-filter app on my computer screen within 1 hour before attempting to fall asleep.</t>
-  </si>
-  <si>
     <t>17. I use as little light as possible when I get up during the night.</t>
   </si>
   <si>
@@ -108,26 +84,50 @@
     <t>04. I spend 30 minutes or less per day (in total) outside.</t>
   </si>
   <si>
-    <t>05. I spend between 1 and 3 hours per day (in total) outside.</t>
-  </si>
-  <si>
-    <t>06. I spend between 30 minutes and 1 hour per day (in total) outside.</t>
-  </si>
-  <si>
-    <t>07.I spend more than 3 hours per day (in total) outside.</t>
-  </si>
-  <si>
-    <t>08.I spend as much time outside as possible.</t>
-  </si>
-  <si>
-    <t>09.I go for a walk or exercise outside within 2 hours after waking up.</t>
+    <t>01. I wear blue-filtering, orange-tinted, and/or red-tinted glasses indoors during the day.</t>
+  </si>
+  <si>
+    <t>02. I wear blue-filtering, orange-tinted, and/or red-tinted glasses outdoors during the day.</t>
+  </si>
+  <si>
+    <t>05. I spend between 30 minutes and 1 hour per day (in total) outside.</t>
+  </si>
+  <si>
+    <t>06. I spend between 1 and 3 hours per day (in total) outside.</t>
+  </si>
+  <si>
+    <t>07. I spend more than 3 hours per day (in total) outside.</t>
+  </si>
+  <si>
+    <t>08. I spend as much time outside as possible.</t>
+  </si>
+  <si>
+    <t>09. I go for a walk or exercise outside within 2 hours after waking up.</t>
+  </si>
+  <si>
+    <t>10. I use my mobile phone within 1 hour before attempting to fall asleep.</t>
+  </si>
+  <si>
+    <t>11. I look at my mobile phone screen immediately after waking up.</t>
+  </si>
+  <si>
+    <t>13. I look at my smartwatch within 1 hour before attempting to fall asleep</t>
+  </si>
+  <si>
+    <t>14. I look at my smartwatch when I wake up at night.</t>
+  </si>
+  <si>
+    <t>15. I dim my mobile phone screen within 1 hour before attempting to fall asleep.</t>
+  </si>
+  <si>
+    <t>16. I use a blue-filter app on my computer screen within 1 hour before attempting to fall asleep.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +140,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,9 +170,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,151 +491,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90301DE1-2331-234C-8755-3BE8A9A5E6F9}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="130.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="136.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" ht="25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>